<commit_message>
Optimizing figures and tables for whole-brain meta-analysis
</commit_message>
<xml_diff>
--- a/F_Meta_Analysis_WholeBrain/figure_results/Hrvrd_Cort_Conservative_pla_g_pperm05.xlsx
+++ b/F_Meta_Analysis_WholeBrain/figure_results/Hrvrd_Cort_Conservative_pla_g_pperm05.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>No</t>
   </si>
@@ -26,10 +26,10 @@
     <t>Frontal Pole (1.2%), Lateral Occipital Cortex, superior division (0.7%)</t>
   </si>
   <si>
-    <t>Temporal Occipital Fusiform Cortex (8.2%), Occipital Fusiform Gyrus (6%)</t>
-  </si>
-  <si>
-    <t>Temporal Occipital Fusiform Cortex (3%), Occipital Fusiform Gyrus (1%)</t>
+    <t>Temporal Occipital Fusiform Cortex (11.8%), Occipital Fusiform Gyrus (5.8%)</t>
+  </si>
+  <si>
+    <t>Insular Cortex (69%)</t>
   </si>
   <si>
     <t>X</t>
@@ -41,7 +41,7 @@
     <t>-40</t>
   </si>
   <si>
-    <t>-46</t>
+    <t>38</t>
   </si>
   <si>
     <t>Y</t>
@@ -50,7 +50,10 @@
     <t>-126</t>
   </si>
   <si>
-    <t>-64</t>
+    <t>-62</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>Z</t>
@@ -62,7 +65,7 @@
     <t>-24</t>
   </si>
   <si>
-    <t>-26</t>
+    <t>0</t>
   </si>
   <si>
     <t>Voxels</t>
@@ -71,7 +74,7 @@
     <t>902629</t>
   </si>
   <si>
-    <t>12</t>
+    <t>4</t>
   </si>
   <si>
     <t>1</t>
@@ -80,28 +83,22 @@
     <t>n</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>420</t>
-  </si>
-  <si>
-    <t>397</t>
-  </si>
-  <si>
-    <t>Isq</t>
-  </si>
-  <si>
-    <t>0%</t>
+    <t>409</t>
+  </si>
+  <si>
+    <t>415</t>
+  </si>
+  <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>0.00</t>
   </si>
   <si>
     <t>g</t>
   </si>
   <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>-0.20</t>
+    <t>-0.19</t>
   </si>
   <si>
     <t>-0.17</t>
@@ -113,28 +110,28 @@
     <t>0.05</t>
   </si>
   <si>
+    <t>0.04</t>
+  </si>
+  <si>
     <t>z</t>
   </si>
   <si>
-    <t>-4.18</t>
-  </si>
-  <si>
-    <t>-3.78</t>
-  </si>
-  <si>
-    <t>p001_uncorr</t>
+    <t>-3.89</t>
+  </si>
+  <si>
+    <t>-3.84</t>
+  </si>
+  <si>
+    <t>p05perm</t>
   </si>
   <si>
     <t>&lt;.001</t>
   </si>
   <si>
-    <t>p05perm</t>
-  </si>
-  <si>
-    <t>.008</t>
-  </si>
-  <si>
-    <t>.045</t>
+    <t>.034</t>
+  </si>
+  <si>
+    <t>.043</t>
   </si>
 </sst>
 </file>
@@ -155,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -165,26 +162,14 @@
     </border>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,103 +179,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="true"/>
-    <col min="2" max="2" width="72.7109375" customWidth="true"/>
+    <col min="2" max="2" width="75.7109375" customWidth="true"/>
     <col min="3" max="3" width="3.7109375" customWidth="true"/>
     <col min="4" max="4" width="4.7109375" customWidth="true"/>
     <col min="5" max="5" width="3.7109375" customWidth="true"/>
     <col min="6" max="6" width="6.7109375" customWidth="true"/>
     <col min="7" max="7" width="3.7109375" customWidth="true"/>
-    <col min="8" max="8" width="3.7109375" customWidth="true"/>
+    <col min="8" max="8" width="4.7109375" customWidth="true"/>
     <col min="9" max="9" width="5.7109375" customWidth="true"/>
     <col min="10" max="10" width="4.7109375" customWidth="true"/>
     <col min="11" max="11" width="5.7109375" customWidth="true"/>
     <col min="12" max="12" width="7.7109375" customWidth="true"/>
-    <col min="13" max="13" width="7.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="7" t="s">
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>37</v>
+      <c r="L1" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="5" t="s">
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -298,82 +276,76 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="7" t="s">
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>38</v>
+      <c r="L3" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="7" t="s">
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>39</v>
+      <c r="L4" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>